<commit_message>
Remove display flicker. Change character designs.
</commit_message>
<xml_diff>
--- a/src/Arduino/smeter-design.xlsx
+++ b/src/Arduino/smeter-design.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="14">
   <si>
     <t>.</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>CHAR_7</t>
-  </si>
-  <si>
-    <t>Full block is character 0x111111, rom code A02 (see datasheet)</t>
   </si>
 </sst>
 </file>
@@ -218,8 +215,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -341,7 +342,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +383,8 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -422,9 +425,935 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="195">
+  <dxfs count="279">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -2897,10 +3826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BT47"/>
+  <dimension ref="A2:BL47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="AR68" sqref="AR68"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5230,7 +6159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:72">
+    <row r="33" spans="2:64">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
@@ -5401,7 +6330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:72">
+    <row r="34" spans="2:64">
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
@@ -5572,7 +6501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="2:72">
+    <row r="35" spans="2:64">
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
@@ -5743,7 +6672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:72">
+    <row r="36" spans="2:64">
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
@@ -5914,7 +6843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:72">
+    <row r="37" spans="2:64">
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
@@ -6062,7 +6991,7 @@
       </c>
       <c r="BL37" s="2"/>
     </row>
-    <row r="39" spans="2:72">
+    <row r="39" spans="2:64">
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
         <v>2</v>
@@ -6135,11 +7064,8 @@
       <c r="BJ39" s="3"/>
       <c r="BK39" s="3"/>
       <c r="BL39" s="2"/>
-      <c r="BN39" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="40" spans="2:72">
+    <row r="40" spans="2:64">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -6287,51 +7213,29 @@
       <c r="BD40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE40" s="2"/>
       <c r="BF40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="BG40" s="5">
-        <v>0</v>
-      </c>
-      <c r="BH40" s="5">
-        <v>0</v>
-      </c>
-      <c r="BI40" s="5">
-        <v>0</v>
-      </c>
-      <c r="BJ40" s="5">
-        <v>0</v>
-      </c>
-      <c r="BK40" s="5">
-        <v>0</v>
+      <c r="BG40" s="11">
+        <v>1</v>
+      </c>
+      <c r="BH40" s="11">
+        <v>1</v>
+      </c>
+      <c r="BI40" s="11">
+        <v>1</v>
+      </c>
+      <c r="BJ40" s="11">
+        <v>1</v>
+      </c>
+      <c r="BK40" s="11">
+        <v>1</v>
       </c>
       <c r="BL40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO40" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP40" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ40" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR40" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS40" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT40" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="41" spans="2:72">
+    <row r="41" spans="2:64">
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
@@ -6461,25 +7365,24 @@
       <c r="AX41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AY41" s="8">
-        <v>0</v>
-      </c>
-      <c r="AZ41" s="8">
-        <v>0</v>
-      </c>
-      <c r="BA41" s="8">
-        <v>0</v>
-      </c>
-      <c r="BB41" s="8">
-        <v>0</v>
-      </c>
-      <c r="BC41" s="8">
-        <v>0</v>
+      <c r="AY41" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ41" s="11">
+        <v>1</v>
+      </c>
+      <c r="BA41" s="11">
+        <v>1</v>
+      </c>
+      <c r="BB41" s="11">
+        <v>1</v>
+      </c>
+      <c r="BC41" s="11">
+        <v>1</v>
       </c>
       <c r="BD41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE41" s="2"/>
       <c r="BF41" s="2" t="s">
         <v>6</v>
       </c>
@@ -6501,29 +7404,8 @@
       <c r="BL41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO41" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP41" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ41" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR41" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS41" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT41" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="42" spans="2:72">
+    <row r="42" spans="2:64">
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
@@ -6632,20 +7514,20 @@
       <c r="AP42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AQ42" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR42" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS42" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT42" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU42" s="5">
-        <v>0</v>
+      <c r="AQ42" s="11">
+        <v>1</v>
+      </c>
+      <c r="AR42" s="11">
+        <v>1</v>
+      </c>
+      <c r="AS42" s="11">
+        <v>1</v>
+      </c>
+      <c r="AT42" s="11">
+        <v>1</v>
+      </c>
+      <c r="AU42" s="11">
+        <v>1</v>
       </c>
       <c r="AV42" s="2" t="s">
         <v>7</v>
@@ -6671,7 +7553,6 @@
       <c r="BD42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE42" s="2"/>
       <c r="BF42" s="2" t="s">
         <v>6</v>
       </c>
@@ -6693,29 +7574,8 @@
       <c r="BL42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO42" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP42" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ42" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR42" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS42" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT42" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="43" spans="2:72">
+    <row r="43" spans="2:64">
       <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
@@ -6803,20 +7663,20 @@
       <c r="AH43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AI43" s="5">
-        <v>0</v>
-      </c>
-      <c r="AJ43" s="5">
-        <v>0</v>
-      </c>
-      <c r="AK43" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL43" s="5">
-        <v>0</v>
-      </c>
-      <c r="AM43" s="5">
-        <v>0</v>
+      <c r="AI43" s="11">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="11">
+        <v>1</v>
+      </c>
+      <c r="AK43" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL43" s="11">
+        <v>1</v>
+      </c>
+      <c r="AM43" s="11">
+        <v>1</v>
       </c>
       <c r="AN43" s="2" t="s">
         <v>7</v>
@@ -6863,7 +7723,6 @@
       <c r="BD43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE43" s="2"/>
       <c r="BF43" s="2" t="s">
         <v>6</v>
       </c>
@@ -6885,29 +7744,8 @@
       <c r="BL43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO43" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP43" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ43" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR43" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS43" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT43" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="44" spans="2:72">
+    <row r="44" spans="2:64">
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
@@ -6974,20 +7812,20 @@
       <c r="Z44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AA44" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD44" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE44" s="5">
-        <v>0</v>
+      <c r="AA44" s="11">
+        <v>1</v>
+      </c>
+      <c r="AB44" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC44" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD44" s="11">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="11">
+        <v>1</v>
       </c>
       <c r="AF44" s="2" t="s">
         <v>7</v>
@@ -7055,7 +7893,6 @@
       <c r="BD44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE44" s="2"/>
       <c r="BF44" s="2" t="s">
         <v>6</v>
       </c>
@@ -7077,29 +7914,8 @@
       <c r="BL44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO44" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP44" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ44" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR44" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS44" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT44" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="45" spans="2:72">
+    <row r="45" spans="2:64">
       <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
@@ -7145,20 +7961,20 @@
       <c r="R45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="5">
-        <v>0</v>
-      </c>
-      <c r="T45" s="5">
-        <v>0</v>
-      </c>
-      <c r="U45" s="5">
-        <v>0</v>
-      </c>
-      <c r="V45" s="5">
-        <v>0</v>
-      </c>
-      <c r="W45" s="5">
-        <v>0</v>
+      <c r="S45" s="11">
+        <v>1</v>
+      </c>
+      <c r="T45" s="11">
+        <v>1</v>
+      </c>
+      <c r="U45" s="11">
+        <v>1</v>
+      </c>
+      <c r="V45" s="11">
+        <v>1</v>
+      </c>
+      <c r="W45" s="11">
+        <v>1</v>
       </c>
       <c r="X45" s="2" t="s">
         <v>7</v>
@@ -7247,7 +8063,6 @@
       <c r="BD45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE45" s="2"/>
       <c r="BF45" s="2" t="s">
         <v>6</v>
       </c>
@@ -7269,29 +8084,8 @@
       <c r="BL45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO45" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP45" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ45" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR45" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS45" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT45" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="46" spans="2:72">
+    <row r="46" spans="2:64">
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -7316,20 +8110,20 @@
       <c r="J46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K46" s="5">
-        <v>0</v>
-      </c>
-      <c r="L46" s="5">
-        <v>0</v>
-      </c>
-      <c r="M46" s="5">
-        <v>0</v>
-      </c>
-      <c r="N46" s="5">
-        <v>0</v>
-      </c>
-      <c r="O46" s="5">
-        <v>0</v>
+      <c r="K46" s="11">
+        <v>1</v>
+      </c>
+      <c r="L46" s="11">
+        <v>1</v>
+      </c>
+      <c r="M46" s="11">
+        <v>1</v>
+      </c>
+      <c r="N46" s="11">
+        <v>1</v>
+      </c>
+      <c r="O46" s="11">
+        <v>1</v>
       </c>
       <c r="P46" s="2" t="s">
         <v>7</v>
@@ -7439,7 +8233,6 @@
       <c r="BD46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BE46" s="2"/>
       <c r="BF46" s="2" t="s">
         <v>6</v>
       </c>
@@ -7461,46 +8254,25 @@
       <c r="BL46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="BN46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO46" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP46" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ46" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR46" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS46" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT46" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="47" spans="2:72">
+    <row r="47" spans="2:64">
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="5">
-        <v>0</v>
-      </c>
-      <c r="D47" s="5">
-        <v>0</v>
-      </c>
-      <c r="E47" s="5">
-        <v>1</v>
-      </c>
-      <c r="F47" s="5">
-        <v>0</v>
-      </c>
-      <c r="G47" s="5">
-        <v>0</v>
+      <c r="C47" s="11">
+        <v>1</v>
+      </c>
+      <c r="D47" s="11">
+        <v>1</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
+        <v>1</v>
+      </c>
+      <c r="G47" s="11">
+        <v>1</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>6</v>
@@ -7610,7 +8382,6 @@
       <c r="BC47" s="11">
         <v>1</v>
       </c>
-      <c r="BE47" s="2"/>
       <c r="BF47" s="2" t="s">
         <v>6</v>
       </c>
@@ -7630,410 +8401,561 @@
         <v>1</v>
       </c>
       <c r="BL47" s="2"/>
-      <c r="BN47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="BO47" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP47" s="11">
-        <v>1</v>
-      </c>
-      <c r="BQ47" s="11">
-        <v>1</v>
-      </c>
-      <c r="BR47" s="11">
-        <v>1</v>
-      </c>
-      <c r="BS47" s="11">
-        <v>1</v>
-      </c>
-      <c r="BT47" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:BC12">
-    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="197" priority="158" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:G24">
-    <cfRule type="containsText" dxfId="112" priority="109" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="196" priority="151" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K24">
-    <cfRule type="containsText" dxfId="111" priority="108" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="195" priority="150" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:S24 U17:U24">
-    <cfRule type="containsText" dxfId="110" priority="107" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="194" priority="149" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",S17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17:AA24 AC17:AC24 AE17:AE24">
-    <cfRule type="containsText" dxfId="109" priority="106" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="193" priority="148" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L24">
-    <cfRule type="containsText" dxfId="108" priority="105" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="192" priority="147" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",L17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:M24">
-    <cfRule type="containsText" dxfId="107" priority="104" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="191" priority="146" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",M17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:N24">
-    <cfRule type="containsText" dxfId="106" priority="103" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="190" priority="145" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",N17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O24">
-    <cfRule type="containsText" dxfId="105" priority="102" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="189" priority="144" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",O17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17:T24">
-    <cfRule type="containsText" dxfId="104" priority="101" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="188" priority="143" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",T17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V17:V24">
-    <cfRule type="containsText" dxfId="103" priority="100" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="187" priority="142" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",V17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W17:W24">
-    <cfRule type="containsText" dxfId="102" priority="99" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="186" priority="141" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",W17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB17:AB24">
-    <cfRule type="containsText" dxfId="101" priority="98" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="185" priority="140" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AB17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD17:AD24">
-    <cfRule type="containsText" dxfId="100" priority="97" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="184" priority="139" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AD17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:G37">
-    <cfRule type="containsText" dxfId="99" priority="96" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="183" priority="138" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG45:BK45">
-    <cfRule type="containsText" dxfId="98" priority="13" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="182" priority="55" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG42:BK42">
-    <cfRule type="containsText" dxfId="95" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="179" priority="52" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO41:BS41">
-    <cfRule type="containsText" dxfId="93" priority="8" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO47:BS47">
-    <cfRule type="containsText" dxfId="92" priority="7" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO46:BS46">
-    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO45:BS45">
-    <cfRule type="containsText" dxfId="89" priority="5" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO44:BS44">
-    <cfRule type="containsText" dxfId="87" priority="4" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K30:O37">
-    <cfRule type="containsText" dxfId="86" priority="83" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="170" priority="125" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:T37 V30:W37">
-    <cfRule type="containsText" dxfId="85" priority="82" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="169" priority="124" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",T30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA30:AB37 AD30:AD37">
-    <cfRule type="containsText" dxfId="84" priority="81" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="168" priority="123" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ30:AM37">
-    <cfRule type="containsText" dxfId="83" priority="80" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="167" priority="122" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AJ30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR30:AT37">
-    <cfRule type="containsText" dxfId="82" priority="79" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="166" priority="121" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AR30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ30:AZ37 BB30:BC37">
-    <cfRule type="containsText" dxfId="81" priority="78" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="165" priority="120" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AZ30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH30:BH37 BJ30:BJ37">
-    <cfRule type="containsText" dxfId="80" priority="77" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="164" priority="119" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BH30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S30:S37">
-    <cfRule type="containsText" dxfId="79" priority="76" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="163" priority="118" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",S30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO43:BS43">
-    <cfRule type="containsText" dxfId="78" priority="3" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U30:U37">
-    <cfRule type="containsText" dxfId="77" priority="74" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="161" priority="116" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",U30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO42:BS42">
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AC30:AC37">
-    <cfRule type="containsText" dxfId="75" priority="73" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="159" priority="115" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AC30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE30:AE37">
-    <cfRule type="containsText" dxfId="74" priority="72" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="158" priority="114" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AE30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI30:AI37">
-    <cfRule type="containsText" dxfId="73" priority="71" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="157" priority="113" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ30:AQ37">
-    <cfRule type="containsText" dxfId="72" priority="70" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="156" priority="112" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AQ30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU30:AU37">
-    <cfRule type="containsText" dxfId="71" priority="69" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="155" priority="111" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AU30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY30:AY37">
-    <cfRule type="containsText" dxfId="70" priority="68" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="154" priority="110" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AY30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA30:BA37">
-    <cfRule type="containsText" dxfId="69" priority="67" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="153" priority="109" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BA30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG30:BG37">
-    <cfRule type="containsText" dxfId="68" priority="66" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="152" priority="108" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI30:BI37">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="151" priority="107" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BI30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK30:BK37">
-    <cfRule type="containsText" dxfId="66" priority="64" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="150" priority="106" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BK30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:G47">
-    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="149" priority="105" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY43:BC43">
-    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="148" priority="62" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AY43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG46:BK46">
-    <cfRule type="containsText" dxfId="57" priority="14" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="141" priority="56" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG44:BK44">
-    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="138" priority="54" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG43:BK43">
-    <cfRule type="containsText" dxfId="51" priority="11" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="135" priority="53" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:O47">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="129" priority="85" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",K40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:W45">
-    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="128" priority="84" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",S40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA40:AE44">
-    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="127" priority="83" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI40:AM43">
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="126" priority="82" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ40:AU42">
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="125" priority="81" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AQ40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY40:BC41">
-    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="124" priority="80" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AY40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG40:BK40">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="123" priority="79" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",BG40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47:W47">
-    <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="122" priority="78" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",S47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S46:W46">
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="121" priority="77" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",S46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA47:AE47">
-    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="120" priority="76" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AE46">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="119" priority="75" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA45:AE45">
-    <cfRule type="containsText" dxfId="34" priority="32" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="118" priority="74" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AA45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI47:AM47">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="117" priority="73" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI46:AM46">
-    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="116" priority="72" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI45:AM45">
+    <cfRule type="containsText" dxfId="115" priority="71" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI44:AM44">
+    <cfRule type="containsText" dxfId="114" priority="70" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ43:AU43">
+    <cfRule type="containsText" dxfId="113" priority="69" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY42:BC42">
+    <cfRule type="containsText" dxfId="112" priority="68" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG41:BK41">
+    <cfRule type="containsText" dxfId="111" priority="67" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ47:AU47">
+    <cfRule type="containsText" dxfId="110" priority="66" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ46:AU46">
+    <cfRule type="containsText" dxfId="109" priority="65" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ45:AU45">
+    <cfRule type="containsText" dxfId="108" priority="64" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ44:AU44">
+    <cfRule type="containsText" dxfId="107" priority="63" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY44:BC44">
+    <cfRule type="containsText" dxfId="105" priority="61" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY45:BC45">
+    <cfRule type="containsText" dxfId="104" priority="60" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY46:BC46">
+    <cfRule type="containsText" dxfId="103" priority="59" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY47:BC47">
+    <cfRule type="containsText" dxfId="102" priority="58" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG47:BK47">
+    <cfRule type="containsText" dxfId="101" priority="57" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY45:BC45">
+    <cfRule type="containsText" dxfId="83" priority="12" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY42:BC42">
+    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG41:BK41">
+    <cfRule type="containsText" dxfId="79" priority="8" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG47:BK47">
+    <cfRule type="containsText" dxfId="77" priority="7" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG46:BK46">
+    <cfRule type="containsText" dxfId="75" priority="6" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG45:BK45">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG44:BK44">
+    <cfRule type="containsText" dxfId="71" priority="4" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG43:BK43">
+    <cfRule type="containsText" dxfId="69" priority="3" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG42:BK42">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",BG42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ43:AU43">
+    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY46:BC46">
+    <cfRule type="containsText" dxfId="63" priority="13" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY44:BC44">
+    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY43:BC43">
+    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:G47">
+    <cfRule type="containsText" dxfId="57" priority="42" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40:O45">
+    <cfRule type="containsText" dxfId="55" priority="41" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",K40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S40:W44">
+    <cfRule type="containsText" dxfId="53" priority="40" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",S40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA40:AE43">
+    <cfRule type="containsText" dxfId="51" priority="39" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AA40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI40:AM42">
+    <cfRule type="containsText" dxfId="49" priority="38" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ40:AU41">
+    <cfRule type="containsText" dxfId="47" priority="37" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY40:BC40">
+    <cfRule type="containsText" dxfId="45" priority="36" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47:O47">
+    <cfRule type="containsText" dxfId="43" priority="35" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46:O46">
+    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",K46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S47:W47">
+    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",S47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S46:W46">
+    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",S46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S45:W45">
+    <cfRule type="containsText" dxfId="35" priority="31" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",S45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA47:AE47">
+    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AA47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA46:AE46">
     <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AA46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA45:AE45">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AA45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA44:AE44">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AA44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI43:AM43">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ42:AU42">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY41:BC41">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AY41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI47:AM47">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI46:AM46">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AI46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI45:AM45">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AM44">
-    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="13" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AI44)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ43:AU43">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AQ43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY42:BC42">
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AY42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BG41:BK41">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BG41)))</formula>
+  <conditionalFormatting sqref="AQ44:AU44">
+    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ45:AU45">
+    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ46:AU46">
+    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",AQ46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ47:AU47">
-    <cfRule type="containsText" dxfId="26" priority="24" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AQ47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ46:AU46">
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AQ46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ45:AU45">
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AQ45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ44:AU44">
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AQ44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY44:BC44">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AY44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY45:BC45">
-    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AY45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY46:BC46">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",AY46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AY47:BC47">
-    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="3" priority="14" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",AY47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG47:BK47">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BG47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO40:BS40">
+  <conditionalFormatting sqref="BG40:BK40">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",BO40)))</formula>
+      <formula>NOT(ISERROR(SEARCH("1",BG40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>